<commit_message>
phase 2 retesting 2 feb
</commit_message>
<xml_diff>
--- a/MPartner_Phase2 Retesting.xlsx
+++ b/MPartner_Phase2 Retesting.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Product BIS certificate" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="Summary" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">BugReport!$A$4:$M$17</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">FAQ!$A$5:$P$11</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Partner Certificate'!$A$5:$P$9</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Product BIS certificate'!$A$5:$P$11</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="207">
   <si>
     <t xml:space="preserve">Project Name:-&gt;Mpartner Revamp</t>
   </si>
@@ -553,13 +554,13 @@
     <t xml:space="preserve">Low</t>
   </si>
   <si>
+    <t xml:space="preserve">Fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29-01-2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not Fixed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29-01-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New</t>
   </si>
   <si>
     <t xml:space="preserve">FAQs_TC2</t>
@@ -691,10 +692,13 @@
     <t xml:space="preserve">Survey_TC4</t>
   </si>
   <si>
-    <t xml:space="preserve">There should be a confirmation message before closing the survey.  </t>
+    <t xml:space="preserve">Confirmation message before closing the survey  is not coming at question number 15.</t>
   </si>
   <si>
     <t xml:space="preserve">Click on Cancel Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New</t>
   </si>
   <si>
     <t xml:space="preserve">29-01-2026</t>
@@ -728,7 +732,7 @@
     <t xml:space="preserve">UpperMenuHeader_TC1</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Duplicate upper menu header.                                                                                  2) Dealer Management, Reports, Service and Check Warranty upper sub headers are missing.</t>
+    <t xml:space="preserve">1) Dealer Management, Reports, Service and Check Warranty upper sub headers are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">2)https://lh3.googleusercontent.com/-qXz_Uu-1WQo/YBPUnGtzyvI/AAAAAAAAF0M/XUIumkYoLd8h6JgHDn8SU8ThQ5kAvJIWgCK8BGAsYHg/s0/2021-01-29.jpg</t>
@@ -1011,6 +1015,9 @@
     <t xml:space="preserve">To verify the Upper menu header</t>
   </si>
   <si>
+    <t xml:space="preserve">1) Duplicate upper menu header.                                                                                  2) Dealer Management, Reports, Service and Check Warranty upper sub headers are missing.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Some sub headers are Gallery(rename to Luminous Youtube), Dealer Management, Reports, Service Escalation(rename to Service &amp; it is for all service functionality), FAQs, Check Warranty should be shown in the Upper menu header
 </t>
   </si>
@@ -1114,13 +1121,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1202,6 +1210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1392,7 +1406,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1441,10 +1455,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1461,14 +1471,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1553,6 +1563,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1593,18 +1607,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1613,22 +1619,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1653,7 +1663,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1746,18 +1756,22 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="A5:M17 P7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.06640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.33"/>
@@ -1768,12 +1782,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="6.54"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1911,32 +1928,41 @@
       <c r="P5" s="10" t="s">
         <v>27</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C6" s="13" t="n">
+      <c r="C6" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>33</v>
       </c>
       <c r="K6" s="1"/>
@@ -1944,43 +1970,52 @@
       <c r="M6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="16" t="n">
+      <c r="N6" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R6" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C7" s="13" t="n">
+      <c r="C7" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>41</v>
       </c>
       <c r="K7" s="1"/>
@@ -1988,167 +2023,203 @@
       <c r="M7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="16" t="n">
+      <c r="N7" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="Q7" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R7" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C8" s="13" t="n">
+      <c r="C8" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="17"/>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>46</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>47</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R8" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C9" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="17"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="16" t="n">
+      <c r="N9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q9" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R9" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C10" s="13" t="n">
+      <c r="C10" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13" t="s">
         <v>33</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="16" t="n">
+      <c r="N10" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P10" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q10" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R10" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>13675</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C11" s="12" t="n">
         <v>44218</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="17"/>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="17"/>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>47</v>
       </c>
       <c r="K11" s="1"/>
@@ -2156,13 +2227,22 @@
       <c r="M11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="16" t="n">
+      <c r="N11" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R11" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S11" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2195,28 +2275,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="1" sqref="A5:M17 P6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20"/>
+      <c r="A1" s="19"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
@@ -2245,8 +2328,8 @@
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2259,15 +2342,15 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
@@ -2300,226 +2383,273 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="22" t="s">
         <v>27</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C6" s="25" t="n">
+      <c r="C6" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="16" t="n">
+      <c r="N6" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R6" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C7" s="25" t="n">
+      <c r="C7" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>68</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="16" t="n">
+      <c r="N7" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="Q7" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R7" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C8" s="25" t="n">
+      <c r="C8" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14" t="s">
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P8" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R8" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C9" s="25" t="n">
+      <c r="C9" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>68</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="16" t="n">
+      <c r="N9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="Q9" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R9" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="R10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="R11" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:P9"/>
@@ -2547,597 +2677,605 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:M17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="34" t="s">
+      <c r="L4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" s="38" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35" t="s">
+    <row r="5" s="37" customFormat="true" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="35" t="n">
+      <c r="C5" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="35" t="n">
+      <c r="D5" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="35" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="35"/>
-    </row>
-    <row r="6" s="38" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="s">
+      <c r="M5" s="34"/>
+    </row>
+    <row r="6" s="37" customFormat="true" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="35" t="n">
+      <c r="C6" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="35" t="n">
+      <c r="D6" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="35"/>
-    </row>
-    <row r="7" s="38" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="s">
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" s="37" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="35" t="n">
+      <c r="C7" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="35" t="n">
+      <c r="D7" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="35" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" s="38" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="s">
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" s="37" customFormat="true" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="35" t="n">
+      <c r="C8" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="35" t="n">
+      <c r="D8" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="35" t="s">
+      <c r="H8" s="36"/>
+      <c r="I8" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="35"/>
-    </row>
-    <row r="9" s="38" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="s">
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" s="37" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="35" t="n">
+      <c r="C9" s="34" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="35" t="n">
+      <c r="D9" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="L9" s="35" t="s">
+      <c r="L9" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="35"/>
-    </row>
-    <row r="10" s="38" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" s="37" customFormat="true" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="35" t="n">
+      <c r="C10" s="34" t="n">
         <v>6</v>
       </c>
-      <c r="D10" s="35" t="n">
+      <c r="D10" s="34" t="n">
         <v>13744</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35" t="s">
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" s="37" customFormat="true" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="34" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" s="37" customFormat="true" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="34"/>
+    </row>
+    <row r="13" s="37" customFormat="true" ht="214.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="34" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="36"/>
+      <c r="I13" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="34"/>
+    </row>
+    <row r="14" s="37" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="34" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="M14" s="34"/>
+    </row>
+    <row r="15" s="37" customFormat="true" ht="247.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="34" t="n">
+        <v>11</v>
+      </c>
+      <c r="D15" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L15" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="34"/>
+    </row>
+    <row r="16" s="37" customFormat="true" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="34" t="n">
+        <v>12</v>
+      </c>
+      <c r="D16" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" s="34"/>
+    </row>
+    <row r="17" s="37" customFormat="true" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="34" t="n">
+        <v>13</v>
+      </c>
+      <c r="D17" s="34" t="n">
+        <v>13744</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="M10" s="35"/>
-    </row>
-    <row r="11" s="38" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="35" t="n">
-        <v>7</v>
-      </c>
-      <c r="D11" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L11" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="35"/>
-    </row>
-    <row r="12" s="38" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="D12" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M12" s="35"/>
-    </row>
-    <row r="13" s="38" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="35" t="n">
-        <v>9</v>
-      </c>
-      <c r="D13" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M13" s="35"/>
-    </row>
-    <row r="14" s="38" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="35" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L14" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="35"/>
-    </row>
-    <row r="15" s="38" customFormat="true" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="35" t="n">
-        <v>11</v>
-      </c>
-      <c r="D15" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L15" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M15" s="35"/>
-    </row>
-    <row r="16" s="38" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="35" t="n">
-        <v>12</v>
-      </c>
-      <c r="D16" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M16" s="35"/>
-    </row>
-    <row r="17" s="38" customFormat="true" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="35" t="n">
-        <v>13</v>
-      </c>
-      <c r="D17" s="35" t="n">
-        <v>13744</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="M17" s="35"/>
+      <c r="M17" s="34"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:M17">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="New"/>
+        <filter val="Not Fixed"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="6">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:B2"/>
@@ -3158,6 +3296,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3166,30 +3305,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="A5:M17 P7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="3.74"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="15" min="14" style="0" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20"/>
+      <c r="A1" s="19"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
@@ -3232,7 +3373,7 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3263,7 +3404,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="3"/>
@@ -3273,298 +3414,361 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="22" t="s">
         <v>27</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
-        <v>129</v>
+      <c r="A6" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C6" s="25" t="n">
+      <c r="C6" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
-        <v>132</v>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="M6" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="16" t="n">
+      <c r="N6" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="Q6" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R6" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>13675</v>
       </c>
-      <c r="C7" s="25" t="n">
+      <c r="C7" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>68</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="16" t="n">
+      <c r="N7" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" s="16" customFormat="true" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="Q7" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R7" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="16" t="n">
+      <c r="B8" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C8" s="25" t="n">
+      <c r="C8" s="24" t="n">
         <v>44218</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="M8" s="16" t="s">
+      <c r="J8" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P8" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" s="16" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="Q8" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R8" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="16" t="n">
+      <c r="B9" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C9" s="25" t="n">
+      <c r="C9" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="M9" s="16" t="s">
+      <c r="J9" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="M9" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="16" t="n">
+      <c r="N9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" s="16" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="s">
+      <c r="Q9" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R9" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="16" t="n">
+      <c r="B10" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C10" s="25" t="n">
+      <c r="C10" s="24" t="n">
         <v>44218</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="M10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="15" t="n">
+        <v>13744</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R10" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" s="15" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="15" t="n">
+        <v>13675</v>
+      </c>
+      <c r="C11" s="24" t="n">
+        <v>44218</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="M10" s="16" t="s">
+      <c r="F11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="16" t="n">
+      <c r="N11" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P11" s="15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" s="16" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="16" t="n">
-        <v>13675</v>
-      </c>
-      <c r="C11" s="25" t="n">
-        <v>44218</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="M11" s="16" t="s">
+      <c r="Q11" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R11" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S11" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="N11" s="16" t="n">
-        <v>13744</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N12" s="19"/>
-    </row>
-    <row r="13" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="12" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N12" s="18"/>
+    </row>
+    <row r="13" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N16" s="19"/>
-      <c r="O16" s="16"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:P11"/>
@@ -3591,27 +3795,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="1" sqref="A5:M17 P6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="7.08"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3695,7 +3902,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="43"/>
@@ -3746,154 +3953,190 @@
       <c r="M5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="22" t="s">
         <v>27</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="50" t="s">
-        <v>139</v>
+      <c r="A6" s="43" t="s">
+        <v>140</v>
       </c>
       <c r="B6" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C6" s="51" t="n">
+      <c r="C6" s="50" t="n">
         <v>44218</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="52" t="s">
+      <c r="D6" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52" t="s">
-        <v>141</v>
+      <c r="G6" s="52"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51" t="s">
+        <v>142</v>
       </c>
       <c r="K6" s="42"/>
       <c r="L6" s="42"/>
       <c r="M6" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="16" t="n">
+      <c r="N6" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="15" t="s">
         <v>34</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R6" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="75.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="43" t="s">
         <v>109</v>
       </c>
       <c r="B7" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C7" s="51" t="n">
+      <c r="C7" s="50" t="n">
         <v>44218</v>
       </c>
-      <c r="D7" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="52" t="s">
+      <c r="D7" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="52" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="52" t="s">
-        <v>143</v>
+      <c r="J7" s="51" t="s">
+        <v>144</v>
       </c>
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
       <c r="M7" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="16" t="n">
+      <c r="N7" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" s="16" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="50" t="s">
-        <v>144</v>
+      <c r="Q7" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R7" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="43" t="s">
+        <v>145</v>
       </c>
       <c r="B8" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C8" s="51" t="n">
+      <c r="C8" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K8" s="45"/>
       <c r="L8" s="45"/>
       <c r="M8" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" s="16" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="50" t="s">
+      <c r="Q8" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R8" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" s="15" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="43" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C9" s="51" t="n">
+      <c r="C9" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="45" t="s">
@@ -3905,318 +4148,390 @@
       </c>
       <c r="I9" s="45"/>
       <c r="J9" s="45" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K9" s="45"/>
       <c r="L9" s="45"/>
       <c r="M9" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="16" t="n">
+      <c r="N9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" s="16" customFormat="true" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="50" t="s">
-        <v>150</v>
+      <c r="Q9" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R9" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" s="15" customFormat="true" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="43" t="s">
+        <v>151</v>
       </c>
       <c r="B10" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C10" s="51" t="n">
+      <c r="C10" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E10" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K10" s="45"/>
       <c r="L10" s="45"/>
       <c r="M10" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="16" t="n">
+      <c r="N10" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P10" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" s="16" customFormat="true" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50" t="s">
-        <v>154</v>
+      <c r="Q10" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R10" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" s="15" customFormat="true" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="43" t="s">
+        <v>155</v>
       </c>
       <c r="B11" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C11" s="51" t="n">
+      <c r="C11" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="45" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
       <c r="I11" s="45"/>
       <c r="J11" s="45" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K11" s="45"/>
       <c r="L11" s="45"/>
       <c r="M11" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="16" t="n">
+      <c r="N11" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="P11" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" s="16" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="50" t="s">
-        <v>158</v>
+      <c r="Q11" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R11" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" s="15" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="43" t="s">
+        <v>159</v>
       </c>
       <c r="B12" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C12" s="51" t="n">
+      <c r="C12" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G12" s="45"/>
       <c r="H12" s="45" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I12" s="45"/>
       <c r="J12" s="45" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K12" s="45"/>
       <c r="L12" s="45"/>
       <c r="M12" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="N12" s="19" t="n">
+      <c r="N12" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="O12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="P12" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" s="16" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="50" t="s">
-        <v>163</v>
+      <c r="Q12" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R12" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S12" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" s="15" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="43" t="s">
+        <v>164</v>
       </c>
       <c r="B13" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C13" s="51" t="n">
+      <c r="C13" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G13" s="45"/>
       <c r="H13" s="45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I13" s="45"/>
       <c r="J13" s="45" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K13" s="45"/>
       <c r="L13" s="45"/>
       <c r="M13" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="N13" s="16" t="n">
+      <c r="N13" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O13" s="16" t="s">
+      <c r="O13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="P13" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" s="16" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50" t="s">
-        <v>168</v>
+      <c r="Q13" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R13" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" s="15" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="43" t="s">
+        <v>169</v>
       </c>
       <c r="B14" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C14" s="51" t="n">
+      <c r="C14" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G14" s="45"/>
       <c r="H14" s="45" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I14" s="45"/>
       <c r="J14" s="45" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K14" s="45"/>
       <c r="L14" s="45"/>
       <c r="M14" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="16" t="n">
+      <c r="N14" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" s="16" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="50" t="s">
-        <v>117</v>
+      <c r="Q14" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R14" s="16" t="n">
+        <v>44229</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" s="15" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="43" t="s">
+        <v>118</v>
       </c>
       <c r="B15" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C15" s="51" t="n">
+      <c r="C15" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="45" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J15" s="45" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K15" s="45"/>
       <c r="L15" s="45"/>
       <c r="M15" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="16" t="n">
+      <c r="N15" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O15" s="16" t="s">
+      <c r="O15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="P15" s="15" t="s">
         <v>42</v>
       </c>
+      <c r="Q15" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R15" s="16" t="n">
+        <v>44229</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
-        <v>121</v>
+      <c r="A16" s="43" t="s">
+        <v>122</v>
       </c>
       <c r="B16" s="42" t="n">
         <v>13675</v>
       </c>
-      <c r="C16" s="51" t="n">
+      <c r="C16" s="50" t="n">
         <v>44218</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G16" s="42"/>
       <c r="H16" s="45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I16" s="42"/>
       <c r="J16" s="45" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K16" s="42"/>
       <c r="L16" s="42"/>
       <c r="M16" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="N16" s="19" t="n">
+      <c r="N16" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O16" s="16" t="s">
+      <c r="O16" s="15" t="s">
         <v>35</v>
       </c>
       <c r="P16" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="Q16" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R16" s="16" t="n">
+        <v>44229</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="Q17" s="0" t="n">
+        <v>13790</v>
+      </c>
+      <c r="R17" s="16" t="n">
+        <v>44229</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:P16"/>
@@ -4246,16 +4561,16 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="1" sqref="A5:M17 P6"/>
+      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.49"/>
@@ -4263,7 +4578,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20"/>
+      <c r="A1" s="19"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
@@ -4306,7 +4621,7 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -4337,7 +4652,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="3"/>
@@ -4347,203 +4662,203 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" s="16" customFormat="true" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="16" t="n">
+    <row r="6" s="15" customFormat="true" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C6" s="55" t="n">
+      <c r="C6" s="54" t="n">
         <v>44217</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="M6" s="16" t="s">
+      <c r="H6" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="16" t="n">
+      <c r="N6" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" s="16" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="16" t="n">
+    <row r="7" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C7" s="55" t="n">
+      <c r="C7" s="54" t="n">
         <v>44217</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="J7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="N7" s="16" t="n">
+      <c r="H7" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="N7" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" s="16" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="16" t="n">
+    <row r="8" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="15" t="n">
         <v>13675</v>
       </c>
-      <c r="C8" s="55" t="n">
+      <c r="C8" s="54" t="n">
         <v>44217</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="N8" s="19" t="n">
+      <c r="J8" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="N8" s="18" t="n">
         <v>13744</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="O8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" s="16" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="16" t="n">
+      <c r="P8" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="N9" s="16" t="n">
+      <c r="F9" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="N9" s="15" t="n">
         <v>13744</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D1:J1"/>
@@ -4569,164 +4884,164 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="A5:M17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.73046875" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="A1" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="A2" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="B3" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="61" t="s">
-        <v>198</v>
+      <c r="E3" s="60" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="59" t="n">
+      <c r="A4" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="58" t="n">
         <v>11</v>
       </c>
-      <c r="C4" s="59" t="n">
+      <c r="C4" s="58" t="n">
         <v>11</v>
       </c>
-      <c r="D4" s="60" t="n">
-        <v>7</v>
-      </c>
-      <c r="E4" s="61" t="n">
+      <c r="D4" s="59" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="58" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="59" t="n">
+      <c r="C5" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="59" t="n">
+      <c r="D5" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="60" t="n">
+      <c r="E5" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="58" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="58" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="59" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="62" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="59" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="59" t="n">
-        <v>6</v>
-      </c>
-      <c r="D6" s="60" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="61" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="62" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="62" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="63" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="62" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" s="62" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="63" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="64" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="65" t="s">
-        <v>202</v>
+      <c r="H8" s="64" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" s="59" t="n">
+      <c r="A9" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="58" t="n">
         <f aca="false">SUM(B4:B8)</f>
         <v>31</v>
       </c>
-      <c r="C9" s="59" t="n">
+      <c r="C9" s="58" t="n">
         <f aca="false">SUM(C4:C8)</f>
-        <v>30</v>
-      </c>
-      <c r="D9" s="60" t="n">
+        <v>31</v>
+      </c>
+      <c r="D9" s="59" t="n">
         <f aca="false">SUM(D4:D8)</f>
-        <v>20</v>
-      </c>
-      <c r="E9" s="61" t="n">
+        <v>26</v>
+      </c>
+      <c r="E9" s="60" t="n">
         <f aca="false">SUM(E4:E8)</f>
-        <v>10</v>
-      </c>
-      <c r="H9" s="65" t="s">
-        <v>204</v>
+        <v>5</v>
+      </c>
+      <c r="H9" s="64" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>